<commit_message>
feat: Add all project files except README
</commit_message>
<xml_diff>
--- a/sample_data/Business_Process_List.xlsx
+++ b/sample_data/Business_Process_List.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e7040110a676622/ドキュメント/git-projects/jp-localgov-workflow-kit/sample_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{A6B6E34E-45C2-4642-A23B-EEAB8E1C35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75D7C43-AF41-4FCE-B4A6-0A28F53DDDD9}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{A6B6E34E-45C2-4642-A23B-EEAB8E1C35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{504F3015-13D8-4FEC-8D45-98465093C18B}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="448" xr2:uid="{9DA6C4BC-EC3B-4DAA-B62C-4B589AB972BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="448" xr2:uid="{9DA6C4BC-EC3B-4DAA-B62C-4B589AB972BA}"/>
   </bookViews>
   <sheets>
     <sheet name="業務リスト" sheetId="20" r:id="rId1"/>
@@ -2833,5 +2828,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: Add generated flowchart Excel to examples
</commit_message>
<xml_diff>
--- a/sample_data/Business_Process_List.xlsx
+++ b/sample_data/Business_Process_List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{A6B6E34E-45C2-4642-A23B-EEAB8E1C35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{504F3015-13D8-4FEC-8D45-98465093C18B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{A6B6E34E-45C2-4642-A23B-EEAB8E1C35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AECF4A43-D717-4DF4-960D-33F0141E014F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="448" xr2:uid="{9DA6C4BC-EC3B-4DAA-B62C-4B589AB972BA}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="448" xr2:uid="{9DA6C4BC-EC3B-4DAA-B62C-4B589AB972BA}"/>
   </bookViews>
   <sheets>
     <sheet name="業務リスト" sheetId="20" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: Update sample data and example files
</commit_message>
<xml_diff>
--- a/sample_data/Business_Process_List.xlsx
+++ b/sample_data/Business_Process_List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{A6B6E34E-45C2-4642-A23B-EEAB8E1C35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AECF4A43-D717-4DF4-960D-33F0141E014F}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{A6B6E34E-45C2-4642-A23B-EEAB8E1C35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84734206-8EBB-4F3B-982B-E391714A9F8B}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="448" xr2:uid="{9DA6C4BC-EC3B-4DAA-B62C-4B589AB972BA}"/>
   </bookViews>
@@ -164,9 +164,6 @@
     <t>照合結果はOKか？</t>
   </si>
   <si>
-    <t>3回間違えるとロックされる</t>
-  </si>
-  <si>
     <t>交付可能な証明書一覧を表示</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>申請書に必要事項を記入</t>
   </si>
   <si>
-    <t>記入例が分かりにくいとの意見あり</t>
-  </si>
-  <si>
     <t>記入済み申請書を受け取る</t>
   </si>
   <si>
@@ -329,9 +323,6 @@
     <t>内容に問題はないか？</t>
   </si>
   <si>
-    <t>印字かすれ、内容相違など</t>
-  </si>
-  <si>
     <t>最初の担当者に通知</t>
   </si>
   <si>
@@ -356,9 +347,6 @@
     <t>手数料を案内</t>
   </si>
   <si>
-    <t>減免の有無で金額が変わる</t>
-  </si>
-  <si>
     <t>手数料を支払う</t>
   </si>
   <si>
@@ -404,13 +392,7 @@
     <t>内容を確認し、確定</t>
   </si>
   <si>
-    <t>窓口より50円安い250円</t>
-  </si>
-  <si>
     <t>エラーメッセージを表示</t>
-  </si>
-  <si>
-    <t>「暗証番号が違います。残りN回」</t>
   </si>
   <si>
     <t>エラーを確認</t>
@@ -577,6 +559,30 @@
     <rPh sb="16" eb="17">
       <t>ツ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>印字かすれ、内容相違など</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3回間違えるとロックされる</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>窓口より50円安い250円</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「暗証番号が違います。残りN回」</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>記入例が分かりにくい</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>減免の有無で金額が変わる</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1127,7 +1133,7 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -1188,7 +1194,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>15</v>
@@ -1212,7 +1218,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>21</v>
@@ -1220,14 +1226,14 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1238,7 +1244,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>17</v>
@@ -1248,13 +1254,13 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J4" s="7">
         <v>4</v>
@@ -1268,7 +1274,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -1277,16 +1283,16 @@
         <v>19</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J5" s="7">
         <v>5</v>
@@ -1300,7 +1306,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -1309,7 +1315,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
@@ -1338,13 +1344,13 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="I7" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J7" s="7">
         <v>7</v>
@@ -1358,7 +1364,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -1370,7 +1376,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>1</v>
@@ -1388,7 +1394,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -1414,7 +1420,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
@@ -1450,11 +1456,11 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J11" s="7">
         <v>11</v>
@@ -1468,7 +1474,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -1502,12 +1508,12 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1528,7 +1534,7 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>1</v>
@@ -1546,7 +1552,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -1557,13 +1563,13 @@
       <c r="F15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="J15" s="7">
         <v>15</v>
       </c>
@@ -1576,7 +1582,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -1588,7 +1594,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="J16" s="7">
         <v>16</v>
@@ -1602,7 +1608,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>21</v>
@@ -1612,12 +1618,12 @@
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1628,7 +1634,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -1641,7 +1647,7 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="7">
@@ -1656,22 +1662,22 @@
         <v>27</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1682,7 +1688,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -1707,10 +1713,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -1722,10 +1728,10 @@
         <v>35</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="7">
@@ -1738,7 +1744,7 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>23</v>
@@ -1760,7 +1766,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>17</v>
@@ -1774,7 +1780,7 @@
         <v>3</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J23" s="7">
         <v>23</v>
@@ -1788,7 +1794,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -1799,7 +1805,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="7">
@@ -1814,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>17</v>
@@ -1826,7 +1832,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>1</v>
@@ -1844,7 +1850,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>36</v>
@@ -1854,7 +1860,7 @@
         <v>37</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>1</v>
@@ -1872,7 +1878,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -1882,7 +1888,7 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>3</v>
@@ -1900,20 +1906,20 @@
         <v>20</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="F28" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1964,7 +1970,7 @@
         <v>28</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>1</v>
@@ -1982,7 +1988,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>17</v>
@@ -2008,7 +2014,7 @@
         <v>14</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>17</v>
@@ -2032,7 +2038,7 @@
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>23</v>
@@ -2054,7 +2060,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>17</v>
@@ -2064,7 +2070,7 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>3</v>
@@ -2079,10 +2085,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>17</v>
@@ -2108,7 +2114,7 @@
         <v>27</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>17</v>
@@ -2118,7 +2124,7 @@
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2134,7 +2140,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>17</v>
@@ -2146,13 +2152,13 @@
         <v>41</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="J37" s="7">
         <v>37</v>
@@ -2166,7 +2172,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>17</v>
@@ -2192,7 +2198,7 @@
         <v>14</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>17</v>
@@ -2218,7 +2224,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>17</v>
@@ -2242,7 +2248,7 @@
         <v>14</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>17</v>
@@ -2254,7 +2260,7 @@
         <v>43</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>1</v>
@@ -2272,7 +2278,7 @@
         <v>14</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>17</v>
@@ -2320,7 +2326,7 @@
         <v>14</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>17</v>
@@ -2346,14 +2352,14 @@
         <v>43</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -2376,14 +2382,14 @@
         <v>21</v>
       </c>
       <c r="E46" s="6"/>
-      <c r="F46" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2394,7 +2400,7 @@
         <v>43</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>36</v>
@@ -2416,7 +2422,7 @@
         <v>14</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>17</v>
@@ -2442,14 +2448,14 @@
         <v>43</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -2466,7 +2472,7 @@
         <v>14</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>17</v>
@@ -2492,7 +2498,7 @@
         <v>43</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>36</v>
@@ -2514,7 +2520,7 @@
         <v>14</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>17</v>
@@ -2540,16 +2546,16 @@
         <v>43</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E53" s="6"/>
-      <c r="F53" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="7">
@@ -2564,7 +2570,7 @@
         <v>14</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>17</v>
@@ -2576,7 +2582,7 @@
         <v>43</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -2592,16 +2598,16 @@
         <v>43</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E55" s="6"/>
-      <c r="F55" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="7">
@@ -2616,7 +2622,7 @@
         <v>14</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>17</v>
@@ -2640,7 +2646,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>36</v>
@@ -2662,20 +2668,20 @@
         <v>43</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="J58" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2696,7 +2702,7 @@
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -2712,7 +2718,7 @@
         <v>14</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>17</v>
@@ -2734,7 +2740,7 @@
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>23</v>
@@ -2756,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>17</v>
@@ -2780,7 +2786,7 @@
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>23</v>
@@ -2800,14 +2806,14 @@
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D64" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>

</xml_diff>